<commit_message>
Added description in Menu Design
as per summary
</commit_message>
<xml_diff>
--- a/_DOCUMENTS_/Menu Design.xlsx
+++ b/_DOCUMENTS_/Menu Design.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\RoyalPetz\_DOCUMENTS_\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ENG" sheetId="1" r:id="rId1"/>
@@ -18,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="202">
   <si>
     <t>Menu Utama</t>
   </si>
@@ -392,12 +397,6 @@
     <t>Retur Pembelian</t>
   </si>
   <si>
-    <t>Sesuai Data Pemasok</t>
-  </si>
-  <si>
-    <t>Sesuai Produk</t>
-  </si>
-  <si>
     <t>Pelanggan</t>
   </si>
   <si>
@@ -416,18 +415,6 @@
     <t>Tambah/ Hapus Pelanggan</t>
   </si>
   <si>
-    <t>Tambah/ Hapus Transaksi</t>
-  </si>
-  <si>
-    <t>Pengaturan Nomor Faktur</t>
-  </si>
-  <si>
-    <t>Sesuai Nomor Faktur</t>
-  </si>
-  <si>
-    <t>Sesuai Data Pelanggan</t>
-  </si>
-  <si>
     <t>Pengaturan Nomor Akun</t>
   </si>
   <si>
@@ -507,6 +494,141 @@
   </si>
   <si>
     <t>Main Menu</t>
+  </si>
+  <si>
+    <t>mysqldump</t>
+  </si>
+  <si>
+    <t>sekalian add/delete group, sesuai modul, modul disimpan di tabel</t>
+  </si>
+  <si>
+    <t>relasi user ke group, tabel siap untuk one to many, tp aplikasi sekarang one to one</t>
+  </si>
+  <si>
+    <t>control panel -&gt; devices and printers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tambah/hapus produk bisa link ke pengaturan harga jual, limit stok, pecah satuan produk </t>
+  </si>
+  <si>
+    <t>tidak perlu tabel terpisah, dijadikan satu di produk, input dibagi 2 , kode rak (C), dan nomor lorong (1)</t>
+  </si>
+  <si>
+    <t>ini group diskon, diskon berupa persen (perbarang), customer dan group customer, hubungan one to one</t>
+  </si>
+  <si>
+    <t>tanpa harga mark up, cuma ada HPP dan HEP (harga tertinggi)</t>
+  </si>
+  <si>
+    <t>multiple limit stok untuk multiple produk</t>
+  </si>
+  <si>
+    <t>ini sekedar informasi, isinya berarti tag dan deskripsi, barang dengan kategori hubungan one to many. dr detail kategori ke produk</t>
+  </si>
+  <si>
+    <t>ini pilih produk dulu, baru pecah, ada akses buat masuk ke tambah/hapus produk</t>
+  </si>
+  <si>
+    <t>input nama satuan dan deskripsi</t>
+  </si>
+  <si>
+    <t>hubungan many to one, banyak satuan ke satuan terkecil</t>
+  </si>
+  <si>
+    <t>transaksi penyesuaian, isinya penyesuaian tiap produk, user input nilai deviasi bisa positif, bisa negatif</t>
+  </si>
+  <si>
+    <t>input ip, bisa localhost bisa ip tertentu</t>
+  </si>
+  <si>
+    <t>Ke Branch</t>
+  </si>
+  <si>
+    <t>input nama kategori dan deskripsi, flag untuk menentukan efek global atau lokal</t>
+  </si>
+  <si>
+    <t>bisa USB Export bisa Online, yg disinkronisasi informasi produk termasuk kategori produk itu, master unit, master kategori</t>
+  </si>
+  <si>
+    <t>permintaan produk ke pusat / cabang bisa via USB export</t>
+  </si>
+  <si>
+    <t>Request Ulang Permintaan Produk</t>
+  </si>
+  <si>
+    <t>Mutasi Barang</t>
+  </si>
+  <si>
+    <t>langsung input ke tabel mutasi ke tempat yg dituju, sekaligus insert ke tabel penerimaan</t>
+  </si>
+  <si>
+    <t>Import Data USB untuk Mutasi</t>
+  </si>
+  <si>
+    <t>Accept / Decline request</t>
+  </si>
+  <si>
+    <t>Sinkronisasi Informasi</t>
+  </si>
+  <si>
+    <t>pilih retur kemana, misalkan cabang berarti retur ke HO, klo HO berarti retur ke supplier</t>
+  </si>
+  <si>
+    <t>simpan HPP, HPP default ambil dr tabel, editable</t>
+  </si>
+  <si>
+    <t>MODUL KASIR</t>
+  </si>
+  <si>
+    <t>By Stock Adjustment</t>
+  </si>
+  <si>
+    <t>ada prompt dengan level yg bisa akses stock adjustment</t>
+  </si>
+  <si>
+    <t>Search penjualan untuk mencari invoice, baru input data retur, retur ada tabel sendiri untuk cross check ke invoice</t>
+  </si>
+  <si>
+    <t>Set No Faktur</t>
+  </si>
+  <si>
+    <t>no faktur reset tiap bulan, formate kode awal nota + bulan tahun + no urut</t>
+  </si>
+  <si>
+    <t>Set Cabang</t>
+  </si>
+  <si>
+    <t>data yg dibutuhkan, nama cabang, alamat ip cabang, alamat cabang, no telp, fax, autogenerate kode cabang dari nama cabang</t>
+  </si>
+  <si>
+    <t>input manual, setelah transaksi yg diinput otomatis dari bbrp kode yang sudah ditentukan dr awal</t>
+  </si>
+  <si>
+    <t>pilih no faktur dr supplier, yg sudah diterima di penerimaan barang, baru dikasih flag klo sudah dibayar</t>
+  </si>
+  <si>
+    <t>pilih no invoice yg pembayaran berupa kredit</t>
+  </si>
+  <si>
+    <t>tambah kurang jumlah barang, langsung input ke tabel hutang</t>
+  </si>
+  <si>
+    <t>langsung input ke tabel piutang klo penjualan berupa kredit</t>
+  </si>
+  <si>
+    <t>langsung input ke tabel pajak berdasarkan perhitungan limit</t>
+  </si>
+  <si>
+    <t>input rata2 omset pembelian harian</t>
+  </si>
+  <si>
+    <t>input rata2 omset penjualan harian</t>
+  </si>
+  <si>
+    <t>input berapa persen dr total omset penjualan harian dan penjualan harian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input rasio toleransi </t>
   </si>
 </sst>
 </file>
@@ -551,9 +673,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -563,6 +692,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -611,7 +743,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -646,7 +778,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -860,7 +992,9 @@
   </sheetPr>
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69:E72"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -873,7 +1007,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1318,57 +1452,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="119" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>87</v>
       </c>
       <c r="D5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>90</v>
       </c>
@@ -1376,381 +1523,511 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>104</v>
       </c>
       <c r="D9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>95</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+      <c r="E13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="E14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="E15" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="E16" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="E17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+      <c r="E18" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="E19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>102</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D20" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="E20" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>103</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D21" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D20" t="s">
+      <c r="E21" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="E22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>26</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D22" t="s">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
+      <c r="E24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C28" t="s">
         <v>117</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D28" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>118</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D29" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D26" t="s">
+      <c r="E29" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+      <c r="E32" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>123</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D29" t="s">
+      <c r="D37" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
+      <c r="D40" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
+      <c r="E41" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D42" s="3"/>
+      <c r="E42" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D43" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="E43" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>126</v>
+      </c>
+      <c r="D45" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
+        <v>185</v>
+      </c>
+      <c r="E46" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>131</v>
+      </c>
+      <c r="D49" t="s">
+        <v>132</v>
+      </c>
+      <c r="E49" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>133</v>
+      </c>
+      <c r="E50" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D32" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="E51" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>116</v>
+      </c>
+      <c r="D52" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="E52" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
+      <c r="D57" t="s">
         <v>137</v>
       </c>
-      <c r="D42" t="s">
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D43" t="s">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>124</v>
+      </c>
+      <c r="D60" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C45" t="s">
-        <v>116</v>
-      </c>
-      <c r="D45" t="s">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C47" t="s">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" t="s">
         <v>142</v>
       </c>
-      <c r="D47" t="s">
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D63" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
-        <v>117</v>
-      </c>
-      <c r="D48" t="s">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D64" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D49" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D51" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C52" t="s">
-        <v>95</v>
-      </c>
-      <c r="D52" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D53" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D54" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D55" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D56" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
-        <v>105</v>
-      </c>
-      <c r="D57" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D59" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
-        <v>106</v>
-      </c>
-      <c r="D60" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D61" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D62" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>107</v>
-      </c>
-      <c r="D63" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D64" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D65" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D66" t="s">
-        <v>160</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>105</v>
+      </c>
+      <c r="D67" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C68" t="s">
-        <v>107</v>
-      </c>
       <c r="D68" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>137</v>
-      </c>
       <c r="D69" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>106</v>
+      </c>
       <c r="D70" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D71" t="s">
-        <v>140</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>107</v>
+      </c>
+      <c r="D73" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C78" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>131</v>
+      </c>
+      <c r="D79" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D40:D42"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>